<commit_message>
serialize KV and flow pairs according to its order of appearance
</commit_message>
<xml_diff>
--- a/output/cpc-material-method.xlsx
+++ b/output/cpc-material-method.xlsx
@@ -34,6 +34,18 @@
     <t xml:space="preserve">Preparation and Environment </t>
   </si>
   <si>
+    <t>protonation method</t>
+  </si>
+  <si>
+    <t>PROPKA</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
     <t>step type</t>
   </si>
   <si>
@@ -64,33 +76,21 @@
     <t>true</t>
   </si>
   <si>
+    <t>Lipid type</t>
+  </si>
+  <si>
+    <t>POPC</t>
+  </si>
+  <si>
+    <t>box type</t>
+  </si>
+  <si>
+    <t>rectangular</t>
+  </si>
+  <si>
     <t>false</t>
   </si>
   <si>
-    <t>protonation method</t>
-  </si>
-  <si>
-    <t>PROPKA</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
-    <t>7.4</t>
-  </si>
-  <si>
-    <t>Lipid type</t>
-  </si>
-  <si>
-    <t>POPC</t>
-  </si>
-  <si>
-    <t>box type</t>
-  </si>
-  <si>
-    <t>rectangular</t>
-  </si>
-  <si>
     <t>octahedral</t>
   </si>
   <si>
@@ -106,30 +106,30 @@
     <t>12 Å</t>
   </si>
   <si>
+    <t>simulation</t>
+  </si>
+  <si>
+    <t>molecular dynamics</t>
+  </si>
+  <si>
+    <t>suite</t>
+  </si>
+  <si>
+    <t>AMBER14</t>
+  </si>
+  <si>
+    <t>force field</t>
+  </si>
+  <si>
+    <t>ff14SB</t>
+  </si>
+  <si>
     <t>ELIF</t>
   </si>
   <si>
     <t xml:space="preserve"> OPC</t>
   </si>
   <si>
-    <t>simulation</t>
-  </si>
-  <si>
-    <t>molecular dynamics</t>
-  </si>
-  <si>
-    <t>suite</t>
-  </si>
-  <si>
-    <t>AMBER14</t>
-  </si>
-  <si>
-    <t>force field</t>
-  </si>
-  <si>
-    <t>ff14SB</t>
-  </si>
-  <si>
     <t>ff19SB</t>
   </si>
   <si>
@@ -160,6 +160,12 @@
     <t>Minimization</t>
   </si>
   <si>
+    <t>maxcyc</t>
+  </si>
+  <si>
+    <t>17,500</t>
+  </si>
+  <si>
     <t>iteration</t>
   </si>
   <si>
@@ -169,12 +175,6 @@
     <t>cycles of minimization print</t>
   </si>
   <si>
-    <t>maxcyc</t>
-  </si>
-  <si>
-    <t>17,500</t>
-  </si>
-  <si>
     <t>2500</t>
   </si>
   <si>
@@ -193,34 +193,34 @@
     <t>Thermalization</t>
   </si>
   <si>
+    <t>simulation time</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>nstlim</t>
+  </si>
+  <si>
+    <t>12,500</t>
+  </si>
+  <si>
     <t>ntp</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>NVT</t>
+  </si>
+  <si>
     <t>elif</t>
   </si>
   <si>
     <t>gt</t>
-  </si>
-  <si>
-    <t>simulation time</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>nstlim</t>
-  </si>
-  <si>
-    <t>12,500</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
-    <t>NVT</t>
   </si>
   <si>
     <t>NPT</t>
@@ -691,10 +691,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -702,10 +702,10 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -713,10 +713,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -724,10 +724,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -735,10 +735,10 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -746,10 +746,10 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -757,10 +757,10 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -768,10 +768,10 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -779,10 +779,10 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -790,10 +790,10 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -801,10 +801,10 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -812,10 +812,10 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -823,10 +823,10 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -834,7 +834,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
         <v>24</v>
@@ -845,7 +845,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
@@ -878,10 +878,10 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -889,10 +889,10 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -903,7 +903,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -925,7 +925,7 @@
         <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -933,10 +933,10 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -944,10 +944,10 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -955,10 +955,10 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -966,10 +966,10 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -977,10 +977,10 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -988,10 +988,10 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -999,10 +999,10 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1010,10 +1010,10 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1021,10 +1021,10 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1032,10 +1032,10 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1043,10 +1043,10 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1054,10 +1054,10 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1065,10 +1065,10 @@
         <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C42" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1076,10 +1076,10 @@
         <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1098,10 +1098,10 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1109,10 +1109,10 @@
         <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1120,10 +1120,10 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1131,10 +1131,10 @@
         <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C48" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1142,10 +1142,10 @@
         <v>5</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1153,10 +1153,10 @@
         <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1164,10 +1164,10 @@
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1200,7 +1200,7 @@
         <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1208,10 +1208,10 @@
         <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="C55" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1219,10 +1219,10 @@
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C56" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1263,10 +1263,10 @@
         <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C60" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1274,10 +1274,10 @@
         <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1285,10 +1285,10 @@
         <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1296,7 +1296,7 @@
         <v>8</v>
       </c>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="C63" t="s">
         <v>52</v>
@@ -1307,7 +1307,7 @@
         <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C64" t="s">
         <v>53</v>
@@ -1351,10 +1351,10 @@
         <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="C68" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1362,10 +1362,10 @@
         <v>10</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="C69" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1373,10 +1373,10 @@
         <v>10</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C70" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1384,10 +1384,10 @@
         <v>10</v>
       </c>
       <c r="B71" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C71" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1395,10 +1395,10 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1406,10 +1406,10 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C73" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1417,10 +1417,10 @@
         <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C74" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1428,10 +1428,10 @@
         <v>10</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C75" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1439,10 +1439,10 @@
         <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="C76" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1450,10 +1450,10 @@
         <v>10</v>
       </c>
       <c r="B77" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C77" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1461,10 +1461,10 @@
         <v>10</v>
       </c>
       <c r="B78" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="C78" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1472,10 +1472,10 @@
         <v>10</v>
       </c>
       <c r="B79" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="C79" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1483,10 +1483,10 @@
         <v>10</v>
       </c>
       <c r="B80" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -1494,7 +1494,7 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="C81" t="s">
         <v>68</v>
@@ -1505,10 +1505,10 @@
         <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="C82" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1516,7 +1516,7 @@
         <v>10</v>
       </c>
       <c r="B83" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C83" t="s">
         <v>69</v>
@@ -1538,7 +1538,7 @@
         <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C85" t="s">
         <v>72</v>
@@ -1549,7 +1549,7 @@
         <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C86" t="s">
         <v>73</v>
@@ -1615,10 +1615,10 @@
         <v>12</v>
       </c>
       <c r="B92" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="C92" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
     </row>
     <row r="93" spans="1:3">
@@ -1626,10 +1626,10 @@
         <v>12</v>
       </c>
       <c r="B93" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="C93" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1637,10 +1637,10 @@
         <v>12</v>
       </c>
       <c r="B94" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C94" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="95" spans="1:3">
@@ -1648,10 +1648,10 @@
         <v>12</v>
       </c>
       <c r="B95" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C95" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1659,10 +1659,10 @@
         <v>12</v>
       </c>
       <c r="B96" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -1670,10 +1670,10 @@
         <v>12</v>
       </c>
       <c r="B97" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C97" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1681,10 +1681,10 @@
         <v>12</v>
       </c>
       <c r="B98" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C98" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -1692,10 +1692,10 @@
         <v>12</v>
       </c>
       <c r="B99" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C99" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="100" spans="1:3">
@@ -1703,10 +1703,10 @@
         <v>12</v>
       </c>
       <c r="B100" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="C100" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -1714,10 +1714,10 @@
         <v>12</v>
       </c>
       <c r="B101" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C101" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -1725,10 +1725,10 @@
         <v>12</v>
       </c>
       <c r="B102" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="C102" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" spans="1:3">
@@ -1736,10 +1736,10 @@
         <v>12</v>
       </c>
       <c r="B103" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -1747,10 +1747,10 @@
         <v>12</v>
       </c>
       <c r="B104" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C104" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -1758,7 +1758,7 @@
         <v>12</v>
       </c>
       <c r="B105" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="C105" t="s">
         <v>68</v>
@@ -1769,10 +1769,10 @@
         <v>12</v>
       </c>
       <c r="B106" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="C106" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -1780,7 +1780,7 @@
         <v>12</v>
       </c>
       <c r="B107" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C107" t="s">
         <v>69</v>
@@ -1813,7 +1813,7 @@
         <v>12</v>
       </c>
       <c r="B110" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C110" t="s">
         <v>79</v>
@@ -1824,7 +1824,7 @@
         <v>12</v>
       </c>
       <c r="B111" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C111" t="s">
         <v>80</v>
@@ -1857,10 +1857,10 @@
         <v>14</v>
       </c>
       <c r="B114" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="C114" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -1868,10 +1868,10 @@
         <v>14</v>
       </c>
       <c r="B115" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C115" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -1879,10 +1879,10 @@
         <v>14</v>
       </c>
       <c r="B116" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C116" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -1890,10 +1890,10 @@
         <v>14</v>
       </c>
       <c r="B117" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C117" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -1901,10 +1901,10 @@
         <v>14</v>
       </c>
       <c r="B118" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C118" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -1912,10 +1912,10 @@
         <v>14</v>
       </c>
       <c r="B119" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C119" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -1923,10 +1923,10 @@
         <v>14</v>
       </c>
       <c r="B120" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C120" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -1934,10 +1934,10 @@
         <v>14</v>
       </c>
       <c r="B121" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="C121" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -1945,10 +1945,10 @@
         <v>14</v>
       </c>
       <c r="B122" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C122" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -1956,10 +1956,10 @@
         <v>14</v>
       </c>
       <c r="B123" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C123" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -1967,10 +1967,10 @@
         <v>14</v>
       </c>
       <c r="B124" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="C124" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -1978,7 +1978,7 @@
         <v>14</v>
       </c>
       <c r="B125" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="C125" t="s">
         <v>68</v>
@@ -1989,10 +1989,10 @@
         <v>14</v>
       </c>
       <c r="B126" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="C126" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2000,7 +2000,7 @@
         <v>14</v>
       </c>
       <c r="B127" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C127" t="s">
         <v>69</v>
@@ -2011,7 +2011,7 @@
         <v>14</v>
       </c>
       <c r="B128" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C128" t="s">
         <v>84</v>
@@ -2022,7 +2022,7 @@
         <v>14</v>
       </c>
       <c r="B129" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C129" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
edit/add more formal sop sample from cpc
</commit_message>
<xml_diff>
--- a/output/cpc-material-method.xlsx
+++ b/output/cpc-material-method.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatho\Dropbox\Code\Python\docx-sop-parser\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BFEC58-3532-4184-AE63-7BE37BF7540A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F7A6EE-FE29-4F5B-A355-BB14BADF7616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="86">
   <si>
-    <t>LINE NUMBER</t>
+    <t>PARAGRAPH NUMBER</t>
   </si>
   <si>
     <t>KEY</t>
@@ -284,17 +284,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -322,9 +313,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,18 +655,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B93" sqref="A93:B93"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7265625" customWidth="1"/>
-    <col min="2" max="2" width="29.26953125" customWidth="1"/>
-    <col min="3" max="3" width="32.36328125" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -687,7 +677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -698,7 +688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -709,7 +699,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -720,7 +710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -731,7 +721,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -742,7 +732,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -753,7 +743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -764,7 +754,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -775,7 +765,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -786,7 +776,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -797,7 +787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -808,7 +798,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -819,7 +809,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -830,7 +820,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -841,7 +831,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -852,7 +842,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -863,7 +853,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -874,7 +864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -885,7 +875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -896,7 +886,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -907,7 +897,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -918,7 +908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -929,7 +919,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -940,7 +930,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -951,7 +941,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -962,7 +952,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -973,7 +963,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -984,7 +974,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -995,7 +985,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1006,7 +996,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1017,7 +1007,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1028,7 +1018,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1039,7 +1029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -1050,7 +1040,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1061,7 +1051,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1072,7 +1062,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1083,7 +1073,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1094,7 +1084,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1105,7 +1095,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1116,7 +1106,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1127,7 +1117,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1138,7 +1128,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1149,7 +1139,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1160,7 +1150,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -1171,7 +1161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -1182,7 +1172,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -1193,7 +1183,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -1204,7 +1194,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -1215,7 +1205,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -1226,7 +1216,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>3</v>
       </c>
@@ -1237,7 +1227,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>3</v>
       </c>
@@ -1248,7 +1238,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>3</v>
       </c>
@@ -1259,7 +1249,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>3</v>
       </c>
@@ -1270,7 +1260,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
@@ -1281,7 +1271,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
@@ -1292,7 +1282,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3</v>
       </c>
@@ -1303,7 +1293,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>3</v>
       </c>
@@ -1314,7 +1304,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -1325,7 +1315,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>5</v>
       </c>
@@ -1336,7 +1326,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>5</v>
       </c>
@@ -1347,7 +1337,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>5</v>
       </c>
@@ -1358,7 +1348,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>5</v>
       </c>
@@ -1369,7 +1359,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>5</v>
       </c>
@@ -1380,7 +1370,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>5</v>
       </c>
@@ -1391,7 +1381,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>5</v>
       </c>
@@ -1402,7 +1392,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -1413,7 +1403,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>6</v>
       </c>
@@ -1424,7 +1414,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>6</v>
       </c>
@@ -1435,7 +1425,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>6</v>
       </c>
@@ -1446,7 +1436,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>6</v>
       </c>
@@ -1457,7 +1447,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>6</v>
       </c>
@@ -1468,7 +1458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>6</v>
       </c>
@@ -1479,7 +1469,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>6</v>
       </c>
@@ -1490,7 +1480,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>6</v>
       </c>
@@ -1501,7 +1491,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>6</v>
       </c>
@@ -1512,7 +1502,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>6</v>
       </c>
@@ -1523,7 +1513,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>6</v>
       </c>
@@ -1534,7 +1524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>6</v>
       </c>
@@ -1545,7 +1535,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>6</v>
       </c>
@@ -1556,7 +1546,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>6</v>
       </c>
@@ -1567,7 +1557,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>6</v>
       </c>
@@ -1578,7 +1568,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>6</v>
       </c>
@@ -1589,7 +1579,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>6</v>
       </c>
@@ -1600,7 +1590,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>7</v>
       </c>
@@ -1611,7 +1601,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>7</v>
       </c>
@@ -1622,7 +1612,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>7</v>
       </c>
@@ -1633,7 +1623,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>7</v>
       </c>
@@ -1644,7 +1634,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>7</v>
       </c>
@@ -1655,7 +1645,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>7</v>
       </c>
@@ -1666,7 +1656,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>7</v>
       </c>
@@ -1677,7 +1667,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>8</v>
       </c>
@@ -1688,18 +1678,18 @@
         <v>72</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="1">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
         <v>8</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" t="s">
         <v>61</v>
       </c>
       <c r="C93" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>8</v>
       </c>
@@ -1710,7 +1700,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>8</v>
       </c>
@@ -1721,7 +1711,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>8</v>
       </c>
@@ -1732,7 +1722,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>8</v>
       </c>
@@ -1743,7 +1733,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>8</v>
       </c>
@@ -1754,7 +1744,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>8</v>
       </c>
@@ -1765,7 +1755,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>8</v>
       </c>
@@ -1776,7 +1766,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>8</v>
       </c>
@@ -1787,7 +1777,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>8</v>
       </c>
@@ -1798,7 +1788,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>8</v>
       </c>
@@ -1809,7 +1799,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>8</v>
       </c>
@@ -1820,7 +1810,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>8</v>
       </c>
@@ -1831,7 +1821,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>8</v>
       </c>
@@ -1842,7 +1832,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>8</v>
       </c>
@@ -1853,7 +1843,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>8</v>
       </c>
@@ -1864,7 +1854,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>8</v>
       </c>
@@ -1875,7 +1865,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>8</v>
       </c>
@@ -1886,18 +1876,18 @@
         <v>79</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A111" s="1">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111">
         <v>8</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" t="s">
         <v>61</v>
       </c>
       <c r="C111" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>8</v>
       </c>
@@ -1908,7 +1898,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>3</v>
       </c>
@@ -1919,7 +1909,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>9</v>
       </c>
@@ -1930,7 +1920,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>9</v>
       </c>
@@ -1941,7 +1931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>9</v>
       </c>
@@ -1952,7 +1942,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>9</v>
       </c>
@@ -1963,7 +1953,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>9</v>
       </c>
@@ -1974,7 +1964,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>9</v>
       </c>
@@ -1985,7 +1975,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>9</v>
       </c>
@@ -1996,7 +1986,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>9</v>
       </c>
@@ -2007,7 +1997,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>9</v>
       </c>
@@ -2018,7 +2008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>9</v>
       </c>
@@ -2029,7 +2019,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>9</v>
       </c>
@@ -2040,7 +2030,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>9</v>
       </c>
@@ -2051,7 +2041,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>9</v>
       </c>
@@ -2062,7 +2052,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>9</v>
       </c>
@@ -2073,7 +2063,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>9</v>
       </c>
@@ -2084,7 +2074,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>9</v>
       </c>
@@ -2095,7 +2085,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>9</v>
       </c>
@@ -2108,6 +2098,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>